<commit_message>
memulai algoritma naive bayes
</commit_message>
<xml_diff>
--- a/hasil_drop_duplicate_musik_2023_v2.xlsx
+++ b/hasil_drop_duplicate_musik_2023_v2.xlsx
@@ -623,53 +623,53 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Boy's a Liar Pt. 2</t>
+          <t>Fast Car</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Boy's a liar Pt. 2</t>
+          <t>Gettin' Old</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>PinkPantheress</t>
+          <t>Luke Combs</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2023-02-03</t>
+          <t>2023-03-24</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>131013</v>
+        <v>265493</v>
       </c>
       <c r="F4" t="n">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G4" t="n">
-        <v>0.696</v>
+        <v>0.712</v>
       </c>
       <c r="H4" t="n">
-        <v>0.252</v>
+        <v>0.186</v>
       </c>
       <c r="I4" t="n">
-        <v>0.8090000000000001</v>
+        <v>0.603</v>
       </c>
       <c r="J4" t="n">
-        <v>0.000128</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.248</v>
+        <v>0.115</v>
       </c>
       <c r="L4" t="n">
-        <v>-8.254</v>
+        <v>-5.52</v>
       </c>
       <c r="M4" t="n">
-        <v>0.05</v>
+        <v>0.0262</v>
       </c>
       <c r="N4" t="n">
-        <v>132.962</v>
+        <v>97.994</v>
       </c>
       <c r="O4" t="n">
         <v>4</v>
@@ -678,53 +678,53 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Fast Car</t>
+          <t>Boy's a Liar Pt. 2</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Gettin' Old</t>
+          <t>Boy's a liar Pt. 2</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Luke Combs</t>
+          <t>PinkPantheress</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2023-03-24</t>
+          <t>2023-02-03</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>265493</v>
+        <v>131013</v>
       </c>
       <c r="F5" t="n">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="G5" t="n">
-        <v>0.712</v>
+        <v>0.696</v>
       </c>
       <c r="H5" t="n">
-        <v>0.186</v>
+        <v>0.252</v>
       </c>
       <c r="I5" t="n">
-        <v>0.603</v>
+        <v>0.8090000000000001</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>0.000128</v>
       </c>
       <c r="K5" t="n">
-        <v>0.115</v>
+        <v>0.248</v>
       </c>
       <c r="L5" t="n">
-        <v>-5.52</v>
+        <v>-8.254</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0262</v>
+        <v>0.05</v>
       </c>
       <c r="N5" t="n">
-        <v>97.994</v>
+        <v>132.962</v>
       </c>
       <c r="O5" t="n">
         <v>4</v>
@@ -810,7 +810,7 @@
         <v>163854</v>
       </c>
       <c r="F7" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G7" t="n">
         <v>0.517</v>
@@ -1063,163 +1063,163 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PRC</t>
+          <t>All My Life (feat. J. Cole)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>PRC</t>
+          <t>All My Life (feat. J. Cole)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Peso Pluma</t>
+          <t>Lil Durk</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2023-01-23</t>
+          <t>2023-05-12</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>184066</v>
+        <v>223878</v>
       </c>
       <c r="F12" t="n">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G12" t="n">
-        <v>0.784</v>
+        <v>0.829</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0965</v>
+        <v>0.15</v>
       </c>
       <c r="I12" t="n">
-        <v>0.826</v>
+        <v>0.436</v>
       </c>
       <c r="J12" t="n">
-        <v>7.09e-05</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.123</v>
+        <v>0.0954</v>
       </c>
       <c r="L12" t="n">
-        <v>-6.34</v>
+        <v>-8.205</v>
       </c>
       <c r="M12" t="n">
-        <v>0.0538</v>
+        <v>0.327</v>
       </c>
       <c r="N12" t="n">
-        <v>138.078</v>
+        <v>143.031</v>
       </c>
       <c r="O12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>All My Life (feat. J. Cole)</t>
+          <t>PRC</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>All My Life (feat. J. Cole)</t>
+          <t>PRC</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Lil Durk</t>
+          <t>Peso Pluma</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2023-05-12</t>
+          <t>2023-01-23</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>223878</v>
+        <v>184066</v>
       </c>
       <c r="F13" t="n">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G13" t="n">
-        <v>0.829</v>
+        <v>0.784</v>
       </c>
       <c r="H13" t="n">
-        <v>0.15</v>
+        <v>0.0965</v>
       </c>
       <c r="I13" t="n">
-        <v>0.436</v>
+        <v>0.826</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>7.09e-05</v>
       </c>
       <c r="K13" t="n">
-        <v>0.0954</v>
+        <v>0.123</v>
       </c>
       <c r="L13" t="n">
-        <v>-8.205</v>
+        <v>-6.34</v>
       </c>
       <c r="M13" t="n">
-        <v>0.327</v>
+        <v>0.0538</v>
       </c>
       <c r="N13" t="n">
-        <v>143.031</v>
+        <v>138.078</v>
       </c>
       <c r="O13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Thinkin’ Bout Me</t>
+          <t>Stand By Me (feat. Morgan Wallen)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>One Thing At A Time</t>
+          <t>Almost Healed</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Morgan Wallen</t>
+          <t>Lil Durk</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2023-03-03</t>
+          <t>2023-05-26</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>177387</v>
+        <v>219173</v>
       </c>
       <c r="F14" t="n">
         <v>87</v>
       </c>
       <c r="G14" t="n">
-        <v>0.656</v>
+        <v>0.756</v>
       </c>
       <c r="H14" t="n">
-        <v>0.492</v>
+        <v>0.0592</v>
       </c>
       <c r="I14" t="n">
-        <v>0.757</v>
+        <v>0.582</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>0.117</v>
+        <v>0.161</v>
       </c>
       <c r="L14" t="n">
-        <v>-5.775</v>
+        <v>-7.726</v>
       </c>
       <c r="M14" t="n">
-        <v>0.0308</v>
+        <v>0.0343</v>
       </c>
       <c r="N14" t="n">
-        <v>139.971</v>
+        <v>134.07</v>
       </c>
       <c r="O14" t="n">
         <v>4</v>
@@ -1228,53 +1228,53 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Stand By Me (feat. Morgan Wallen)</t>
+          <t>Thinkin’ Bout Me</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Almost Healed</t>
+          <t>One Thing At A Time</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Lil Durk</t>
+          <t>Morgan Wallen</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2023-05-26</t>
+          <t>2023-03-03</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>219173</v>
+        <v>177387</v>
       </c>
       <c r="F15" t="n">
         <v>87</v>
       </c>
       <c r="G15" t="n">
-        <v>0.756</v>
+        <v>0.656</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0592</v>
+        <v>0.492</v>
       </c>
       <c r="I15" t="n">
-        <v>0.582</v>
+        <v>0.757</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.161</v>
+        <v>0.117</v>
       </c>
       <c r="L15" t="n">
-        <v>-7.726</v>
+        <v>-5.775</v>
       </c>
       <c r="M15" t="n">
-        <v>0.0343</v>
+        <v>0.0308</v>
       </c>
       <c r="N15" t="n">
-        <v>134.07</v>
+        <v>139.971</v>
       </c>
       <c r="O15" t="n">
         <v>4</v>
@@ -1283,53 +1283,53 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Daylight</t>
+          <t>Area Codes</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Daylight</t>
+          <t>Area Codes</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>David Kushner</t>
+          <t>Kali</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2023-04-14</t>
+          <t>2023-03-17</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>212953</v>
+        <v>139325</v>
       </c>
       <c r="F16" t="n">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="G16" t="n">
-        <v>0.508</v>
+        <v>0.823</v>
       </c>
       <c r="H16" t="n">
-        <v>0.83</v>
+        <v>0.0187</v>
       </c>
       <c r="I16" t="n">
-        <v>0.43</v>
+        <v>0.388</v>
       </c>
       <c r="J16" t="n">
-        <v>0.000441</v>
+        <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>0.093</v>
+        <v>0.0876</v>
       </c>
       <c r="L16" t="n">
-        <v>-9.475</v>
+        <v>-10.867</v>
       </c>
       <c r="M16" t="n">
-        <v>0.0335</v>
+        <v>0.491</v>
       </c>
       <c r="N16" t="n">
-        <v>130.09</v>
+        <v>154.569</v>
       </c>
       <c r="O16" t="n">
         <v>4</v>
@@ -1338,53 +1338,53 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Area Codes</t>
+          <t>Daylight</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Area Codes</t>
+          <t>Daylight</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Kali</t>
+          <t>David Kushner</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2023-03-17</t>
+          <t>2023-04-14</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>139325</v>
+        <v>212953</v>
       </c>
       <c r="F17" t="n">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="G17" t="n">
-        <v>0.823</v>
+        <v>0.508</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0187</v>
+        <v>0.83</v>
       </c>
       <c r="I17" t="n">
-        <v>0.388</v>
+        <v>0.43</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>0.000441</v>
       </c>
       <c r="K17" t="n">
-        <v>0.0876</v>
+        <v>0.093</v>
       </c>
       <c r="L17" t="n">
-        <v>-10.867</v>
+        <v>-9.475</v>
       </c>
       <c r="M17" t="n">
-        <v>0.491</v>
+        <v>0.0335</v>
       </c>
       <c r="N17" t="n">
-        <v>154.569</v>
+        <v>130.09</v>
       </c>
       <c r="O17" t="n">
         <v>4</v>
@@ -1448,53 +1448,53 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Flowers</t>
+          <t>You Proof</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Flowers</t>
+          <t>One Thing At A Time</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Miley Cyrus</t>
+          <t>Morgan Wallen</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2023-01-13</t>
+          <t>2023-03-03</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>200454</v>
+        <v>157477</v>
       </c>
       <c r="F19" t="n">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G19" t="n">
-        <v>0.707</v>
+        <v>0.732</v>
       </c>
       <c r="H19" t="n">
-        <v>0.06320000000000001</v>
+        <v>0.265</v>
       </c>
       <c r="I19" t="n">
-        <v>0.681</v>
+        <v>0.839</v>
       </c>
       <c r="J19" t="n">
-        <v>5.15e-06</v>
+        <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0322</v>
+        <v>0.602</v>
       </c>
       <c r="L19" t="n">
-        <v>-4.325</v>
+        <v>-5.007</v>
       </c>
       <c r="M19" t="n">
-        <v>0.0668</v>
+        <v>0.0345</v>
       </c>
       <c r="N19" t="n">
-        <v>117.999</v>
+        <v>119.724</v>
       </c>
       <c r="O19" t="n">
         <v>4</v>
@@ -1503,53 +1503,53 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>You Proof</t>
+          <t>Flowers</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>One Thing At A Time</t>
+          <t>Flowers</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Morgan Wallen</t>
+          <t>Miley Cyrus</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2023-03-03</t>
+          <t>2023-01-13</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>157477</v>
+        <v>200454</v>
       </c>
       <c r="F20" t="n">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="G20" t="n">
-        <v>0.732</v>
+        <v>0.707</v>
       </c>
       <c r="H20" t="n">
-        <v>0.265</v>
+        <v>0.06320000000000001</v>
       </c>
       <c r="I20" t="n">
-        <v>0.839</v>
+        <v>0.681</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>5.15e-06</v>
       </c>
       <c r="K20" t="n">
-        <v>0.602</v>
+        <v>0.0322</v>
       </c>
       <c r="L20" t="n">
-        <v>-5.007</v>
+        <v>-4.325</v>
       </c>
       <c r="M20" t="n">
-        <v>0.0345</v>
+        <v>0.0668</v>
       </c>
       <c r="N20" t="n">
-        <v>119.724</v>
+        <v>117.999</v>
       </c>
       <c r="O20" t="n">
         <v>4</v>
@@ -1558,108 +1558,108 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Calling (Spider-Man: Across the Spider-Verse) (Metro Boomin &amp; Swae Lee, NAV, feat. A Boogie Wit da Hoodie)</t>
+          <t>TQM</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>METRO BOOMIN PRESENTS SPIDER-MAN: ACROSS THE SPIDER-VERSE (SOUNDTRACK FROM AND INSPIRED BY THE MOTION PICTURE)</t>
+          <t>TQM</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Metro Boomin</t>
+          <t>Fuerza Regida</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2023-06-02</t>
+          <t>2023-05-19</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>219453</v>
+        <v>158965</v>
       </c>
       <c r="F21" t="n">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G21" t="n">
-        <v>0.631</v>
+        <v>0.786</v>
       </c>
       <c r="H21" t="n">
-        <v>0.464</v>
+        <v>0.273</v>
       </c>
       <c r="I21" t="n">
-        <v>0.535</v>
+        <v>0.853</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
       </c>
       <c r="K21" t="n">
-        <v>0.115</v>
+        <v>0.106</v>
       </c>
       <c r="L21" t="n">
-        <v>-7.836</v>
+        <v>-4.955</v>
       </c>
       <c r="M21" t="n">
-        <v>0.0842</v>
+        <v>0.0589</v>
       </c>
       <c r="N21" t="n">
-        <v>140.127</v>
+        <v>125.107</v>
       </c>
       <c r="O21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>TQM</t>
+          <t>Peso Pluma: Bzrp Music Sessions, Vol. 55</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>TQM</t>
+          <t>Peso Pluma: Bzrp Music Sessions, Vol. 55</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Fuerza Regida</t>
+          <t>Bizarrap</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2023-05-19</t>
+          <t>2023-06-01</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>158965</v>
+        <v>188361</v>
       </c>
       <c r="F22" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G22" t="n">
-        <v>0.786</v>
+        <v>0.854</v>
       </c>
       <c r="H22" t="n">
-        <v>0.273</v>
+        <v>0.264</v>
       </c>
       <c r="I22" t="n">
-        <v>0.853</v>
+        <v>0.668</v>
       </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>5.61e-05</v>
       </c>
       <c r="K22" t="n">
-        <v>0.106</v>
+        <v>0.117</v>
       </c>
       <c r="L22" t="n">
-        <v>-4.955</v>
+        <v>-7.848</v>
       </c>
       <c r="M22" t="n">
-        <v>0.0589</v>
+        <v>0.0466</v>
       </c>
       <c r="N22" t="n">
-        <v>125.107</v>
+        <v>132.966</v>
       </c>
       <c r="O22" t="n">
         <v>3</v>
@@ -1668,7 +1668,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Annihilate (Spider-Man: Across the Spider-Verse) (Metro Boomin &amp; Swae Lee, Lil Wayne, Offset)</t>
+          <t>Calling (Spider-Man: Across the Spider-Verse) (Metro Boomin &amp; Swae Lee, NAV, feat. A Boogie Wit da Hoodie)</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1687,34 +1687,34 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>231746</v>
+        <v>219453</v>
       </c>
       <c r="F23" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G23" t="n">
-        <v>0.611</v>
+        <v>0.631</v>
       </c>
       <c r="H23" t="n">
-        <v>0.214</v>
+        <v>0.464</v>
       </c>
       <c r="I23" t="n">
-        <v>0.483</v>
+        <v>0.535</v>
       </c>
       <c r="J23" t="n">
         <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>0.124</v>
+        <v>0.115</v>
       </c>
       <c r="L23" t="n">
-        <v>-6.216</v>
+        <v>-7.836</v>
       </c>
       <c r="M23" t="n">
-        <v>0.055</v>
+        <v>0.0842</v>
       </c>
       <c r="N23" t="n">
-        <v>145.983</v>
+        <v>140.127</v>
       </c>
       <c r="O23" t="n">
         <v>4</v>
@@ -1723,166 +1723,166 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Ella Baila Sola</t>
+          <t>Annihilate (Spider-Man: Across the Spider-Verse) (Metro Boomin &amp; Swae Lee, Lil Wayne, Offset)</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>DESVELADO</t>
+          <t>METRO BOOMIN PRESENTS SPIDER-MAN: ACROSS THE SPIDER-VERSE (SOUNDTRACK FROM AND INSPIRED BY THE MOTION PICTURE)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Eslabon Armado</t>
+          <t>Metro Boomin</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2023-04-28</t>
+          <t>2023-06-02</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>165671</v>
+        <v>231746</v>
       </c>
       <c r="F24" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G24" t="n">
-        <v>0.668</v>
+        <v>0.611</v>
       </c>
       <c r="H24" t="n">
+        <v>0.214</v>
+      </c>
+      <c r="I24" t="n">
         <v>0.483</v>
       </c>
-      <c r="I24" t="n">
-        <v>0.758</v>
-      </c>
       <c r="J24" t="n">
-        <v>1.89e-05</v>
+        <v>0</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0837</v>
+        <v>0.124</v>
       </c>
       <c r="L24" t="n">
-        <v>-5.176</v>
+        <v>-6.216</v>
       </c>
       <c r="M24" t="n">
-        <v>0.0332</v>
+        <v>0.055</v>
       </c>
       <c r="N24" t="n">
-        <v>147.989</v>
+        <v>145.983</v>
       </c>
       <c r="O24" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>MATHEMATICAL DISRESPECT</t>
+          <t>Ella Baila Sola</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>MATHEMATICAL DISRESPECT</t>
+          <t>DESVELADO</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Lil Mabu</t>
+          <t>Eslabon Armado</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2023-05-05</t>
+          <t>2023-04-28</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>88304</v>
+        <v>165671</v>
       </c>
       <c r="F25" t="n">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="G25" t="n">
-        <v>0.795</v>
+        <v>0.668</v>
       </c>
       <c r="H25" t="n">
-        <v>0.0612</v>
+        <v>0.483</v>
       </c>
       <c r="I25" t="n">
-        <v>0.507</v>
+        <v>0.758</v>
       </c>
       <c r="J25" t="n">
-        <v>0</v>
+        <v>1.89e-05</v>
       </c>
       <c r="K25" t="n">
-        <v>0.272</v>
+        <v>0.0837</v>
       </c>
       <c r="L25" t="n">
-        <v>-8.06</v>
+        <v>-5.176</v>
       </c>
       <c r="M25" t="n">
-        <v>0.303</v>
+        <v>0.0332</v>
       </c>
       <c r="N25" t="n">
-        <v>146.771</v>
+        <v>147.989</v>
       </c>
       <c r="O25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Peso Pluma: Bzrp Music Sessions, Vol. 55</t>
+          <t>MATHEMATICAL DISRESPECT</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Peso Pluma: Bzrp Music Sessions, Vol. 55</t>
+          <t>MATHEMATICAL DISRESPECT</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bizarrap</t>
+          <t>Lil Mabu</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2023-06-01</t>
+          <t>2023-05-05</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>188361</v>
+        <v>88304</v>
       </c>
       <c r="F26" t="n">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G26" t="n">
-        <v>0.854</v>
+        <v>0.795</v>
       </c>
       <c r="H26" t="n">
-        <v>0.264</v>
+        <v>0.0612</v>
       </c>
       <c r="I26" t="n">
-        <v>0.668</v>
+        <v>0.507</v>
       </c>
       <c r="J26" t="n">
-        <v>5.61e-05</v>
+        <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>0.117</v>
+        <v>0.272</v>
       </c>
       <c r="L26" t="n">
-        <v>-7.848</v>
+        <v>-8.06</v>
       </c>
       <c r="M26" t="n">
-        <v>0.0466</v>
+        <v>0.303</v>
       </c>
       <c r="N26" t="n">
-        <v>132.966</v>
+        <v>146.771</v>
       </c>
       <c r="O26" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27">
@@ -1943,53 +1943,53 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Am I Dreaming (Metro Boomin &amp; A$AP Rocky, Roisee)</t>
+          <t>Watch This - ARIZONATEARS Pluggnb Remix</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>METRO BOOMIN PRESENTS SPIDER-MAN: ACROSS THE SPIDER-VERSE (SOUNDTRACK FROM AND INSPIRED BY THE MOTION PICTURE)</t>
+          <t>Watch This (ARIZONATEARS Pluggnb Remix)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Metro Boomin</t>
+          <t>Lil Uzi Vert</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2023-06-02</t>
+          <t>2023-02-05</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>256026</v>
+        <v>163139</v>
       </c>
       <c r="F28" t="n">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G28" t="n">
-        <v>0.599</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="H28" t="n">
-        <v>0.0408</v>
+        <v>0.0103</v>
       </c>
       <c r="I28" t="n">
-        <v>0.526</v>
+        <v>0.897</v>
       </c>
       <c r="J28" t="n">
-        <v>0.00256</v>
+        <v>0.103</v>
       </c>
       <c r="K28" t="n">
-        <v>0.209</v>
+        <v>0.153</v>
       </c>
       <c r="L28" t="n">
-        <v>-7.812</v>
+        <v>-7.18</v>
       </c>
       <c r="M28" t="n">
-        <v>0.0385</v>
+        <v>0.0386</v>
       </c>
       <c r="N28" t="n">
-        <v>90.018</v>
+        <v>129.975</v>
       </c>
       <c r="O28" t="n">
         <v>4</v>
@@ -1998,53 +1998,53 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Watch This - ARIZONATEARS Pluggnb Remix</t>
+          <t>Am I Dreaming (Metro Boomin &amp; A$AP Rocky, Roisee)</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Watch This (ARIZONATEARS Pluggnb Remix)</t>
+          <t>METRO BOOMIN PRESENTS SPIDER-MAN: ACROSS THE SPIDER-VERSE (SOUNDTRACK FROM AND INSPIRED BY THE MOTION PICTURE)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Lil Uzi Vert</t>
+          <t>Metro Boomin</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2023-02-05</t>
+          <t>2023-06-02</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>163139</v>
+        <v>256026</v>
       </c>
       <c r="F29" t="n">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G29" t="n">
-        <v>0.6860000000000001</v>
+        <v>0.599</v>
       </c>
       <c r="H29" t="n">
-        <v>0.0103</v>
+        <v>0.0408</v>
       </c>
       <c r="I29" t="n">
-        <v>0.897</v>
+        <v>0.526</v>
       </c>
       <c r="J29" t="n">
-        <v>0.103</v>
+        <v>0.00256</v>
       </c>
       <c r="K29" t="n">
-        <v>0.153</v>
+        <v>0.209</v>
       </c>
       <c r="L29" t="n">
-        <v>-7.18</v>
+        <v>-7.812</v>
       </c>
       <c r="M29" t="n">
-        <v>0.0386</v>
+        <v>0.0385</v>
       </c>
       <c r="N29" t="n">
-        <v>129.975</v>
+        <v>90.018</v>
       </c>
       <c r="O29" t="n">
         <v>4</v>
@@ -2075,7 +2075,7 @@
         <v>189466</v>
       </c>
       <c r="F30" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G30" t="n">
         <v>0.775</v>
@@ -2163,108 +2163,108 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Favorite Song</t>
+          <t>Bye</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Favorite Song</t>
+          <t>Bye</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Toosii</t>
+          <t>Peso Pluma</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2023-02-17</t>
+          <t>2023-05-26</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>208630</v>
+        <v>212976</v>
       </c>
       <c r="F32" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="G32" t="n">
-        <v>0.8159999999999999</v>
+        <v>0.782</v>
       </c>
       <c r="H32" t="n">
-        <v>0.314</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="I32" t="n">
-        <v>0.367</v>
+        <v>0.8120000000000001</v>
       </c>
       <c r="J32" t="n">
-        <v>0</v>
+        <v>0.00045</v>
       </c>
       <c r="K32" t="n">
-        <v>0.0987</v>
+        <v>0.101</v>
       </c>
       <c r="L32" t="n">
-        <v>-9.353999999999999</v>
+        <v>-6.613</v>
       </c>
       <c r="M32" t="n">
-        <v>0.0588</v>
+        <v>0.0469</v>
       </c>
       <c r="N32" t="n">
-        <v>116.035</v>
+        <v>122.063</v>
       </c>
       <c r="O32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Princess Diana (with Nicki Minaj)</t>
+          <t>Favorite Song</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Princess Diana (with Nicki Minaj)</t>
+          <t>Favorite Song</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Ice Spice</t>
+          <t>Toosii</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2023-04-14</t>
+          <t>2023-02-17</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>172125</v>
+        <v>208630</v>
       </c>
       <c r="F33" t="n">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G33" t="n">
-        <v>0.898</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="H33" t="n">
-        <v>0.14</v>
+        <v>0.314</v>
       </c>
       <c r="I33" t="n">
-        <v>0.676</v>
+        <v>0.367</v>
       </c>
       <c r="J33" t="n">
         <v>0</v>
       </c>
       <c r="K33" t="n">
-        <v>0.101</v>
+        <v>0.0987</v>
       </c>
       <c r="L33" t="n">
-        <v>-5.196</v>
+        <v>-9.353999999999999</v>
       </c>
       <c r="M33" t="n">
-        <v>0.187</v>
+        <v>0.0588</v>
       </c>
       <c r="N33" t="n">
-        <v>147.991</v>
+        <v>116.035</v>
       </c>
       <c r="O33" t="n">
         <v>4</v>
@@ -2273,163 +2273,163 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Chanel</t>
+          <t>Princess Diana (with Nicki Minaj)</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Chanel</t>
+          <t>Princess Diana (with Nicki Minaj)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Becky G</t>
+          <t>Ice Spice</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2023-03-30</t>
+          <t>2023-04-14</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>201993</v>
+        <v>172125</v>
       </c>
       <c r="F34" t="n">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G34" t="n">
-        <v>0.852</v>
+        <v>0.898</v>
       </c>
       <c r="H34" t="n">
-        <v>0.397</v>
+        <v>0.14</v>
       </c>
       <c r="I34" t="n">
-        <v>0.675</v>
+        <v>0.676</v>
       </c>
       <c r="J34" t="n">
-        <v>0.00317</v>
+        <v>0</v>
       </c>
       <c r="K34" t="n">
-        <v>0.0905</v>
+        <v>0.101</v>
       </c>
       <c r="L34" t="n">
-        <v>-5.738</v>
+        <v>-5.196</v>
       </c>
       <c r="M34" t="n">
-        <v>0.0363</v>
+        <v>0.187</v>
       </c>
       <c r="N34" t="n">
-        <v>132.005</v>
+        <v>147.991</v>
       </c>
       <c r="O34" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>TQG</t>
+          <t>Chanel</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>MAÑANA SERÁ BONITO</t>
+          <t>Chanel</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>KAROL G</t>
+          <t>Becky G</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2023-02-24</t>
+          <t>2023-03-30</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>197933</v>
+        <v>201993</v>
       </c>
       <c r="F35" t="n">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G35" t="n">
-        <v>0.72</v>
+        <v>0.852</v>
       </c>
       <c r="H35" t="n">
-        <v>0.673</v>
+        <v>0.397</v>
       </c>
       <c r="I35" t="n">
-        <v>0.63</v>
+        <v>0.675</v>
       </c>
       <c r="J35" t="n">
-        <v>0</v>
+        <v>0.00317</v>
       </c>
       <c r="K35" t="n">
-        <v>0.0936</v>
+        <v>0.0905</v>
       </c>
       <c r="L35" t="n">
-        <v>-3.547</v>
+        <v>-5.738</v>
       </c>
       <c r="M35" t="n">
-        <v>0.277</v>
+        <v>0.0363</v>
       </c>
       <c r="N35" t="n">
-        <v>179.974</v>
+        <v>132.005</v>
       </c>
       <c r="O35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>War Bout It (feat. 21 Savage)</t>
+          <t>TQG</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Almost Healed</t>
+          <t>MAÑANA SERÁ BONITO</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Lil Durk</t>
+          <t>KAROL G</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2023-05-26</t>
+          <t>2023-02-24</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>160202</v>
+        <v>197933</v>
       </c>
       <c r="F36" t="n">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="G36" t="n">
-        <v>0.732</v>
+        <v>0.72</v>
       </c>
       <c r="H36" t="n">
-        <v>0.00385</v>
+        <v>0.673</v>
       </c>
       <c r="I36" t="n">
-        <v>0.6</v>
+        <v>0.63</v>
       </c>
       <c r="J36" t="n">
-        <v>0.000114</v>
+        <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>0.112</v>
+        <v>0.0936</v>
       </c>
       <c r="L36" t="n">
-        <v>-9.057</v>
+        <v>-3.547</v>
       </c>
       <c r="M36" t="n">
-        <v>0.241</v>
+        <v>0.277</v>
       </c>
       <c r="N36" t="n">
-        <v>167.973</v>
+        <v>179.974</v>
       </c>
       <c r="O36" t="n">
         <v>4</v>
@@ -2493,17 +2493,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Bye</t>
+          <t>War Bout It (feat. 21 Savage)</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Bye</t>
+          <t>Almost Healed</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Peso Pluma</t>
+          <t>Lil Durk</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -2512,89 +2512,89 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>212976</v>
+        <v>160202</v>
       </c>
       <c r="F38" t="n">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G38" t="n">
-        <v>0.782</v>
+        <v>0.732</v>
       </c>
       <c r="H38" t="n">
-        <v>0.5669999999999999</v>
+        <v>0.00385</v>
       </c>
       <c r="I38" t="n">
-        <v>0.8120000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="J38" t="n">
-        <v>0.00045</v>
+        <v>0.000114</v>
       </c>
       <c r="K38" t="n">
-        <v>0.101</v>
+        <v>0.112</v>
       </c>
       <c r="L38" t="n">
-        <v>-6.613</v>
+        <v>-9.057</v>
       </c>
       <c r="M38" t="n">
-        <v>0.0469</v>
+        <v>0.241</v>
       </c>
       <c r="N38" t="n">
-        <v>122.063</v>
+        <v>167.973</v>
       </c>
       <c r="O38" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>BESO</t>
+          <t>Cowgirls (feat. ERNEST)</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>RR</t>
+          <t>One Thing At A Time</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>ROSALÍA</t>
+          <t>Morgan Wallen</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2023-03-24</t>
+          <t>2023-03-03</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>194543</v>
+        <v>181621</v>
       </c>
       <c r="F39" t="n">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="G39" t="n">
-        <v>0.768</v>
+        <v>0.624</v>
       </c>
       <c r="H39" t="n">
-        <v>0.736</v>
+        <v>0.199</v>
       </c>
       <c r="I39" t="n">
-        <v>0.644</v>
+        <v>0.766</v>
       </c>
       <c r="J39" t="n">
-        <v>0.000837</v>
+        <v>8.62e-06</v>
       </c>
       <c r="K39" t="n">
-        <v>0.173</v>
+        <v>0.156</v>
       </c>
       <c r="L39" t="n">
-        <v>-6.671</v>
+        <v>-3.805</v>
       </c>
       <c r="M39" t="n">
-        <v>0.136</v>
+        <v>0.0359</v>
       </c>
       <c r="N39" t="n">
-        <v>95.05</v>
+        <v>172.08</v>
       </c>
       <c r="O39" t="n">
         <v>4</v>
@@ -2603,53 +2603,53 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Cowgirls (feat. ERNEST)</t>
+          <t>BESO</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>One Thing At A Time</t>
+          <t>RR</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Morgan Wallen</t>
+          <t>ROSALÍA</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2023-03-03</t>
+          <t>2023-03-24</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>181621</v>
+        <v>194543</v>
       </c>
       <c r="F40" t="n">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="G40" t="n">
-        <v>0.624</v>
+        <v>0.768</v>
       </c>
       <c r="H40" t="n">
-        <v>0.199</v>
+        <v>0.736</v>
       </c>
       <c r="I40" t="n">
-        <v>0.766</v>
+        <v>0.644</v>
       </c>
       <c r="J40" t="n">
-        <v>8.62e-06</v>
+        <v>0.000837</v>
       </c>
       <c r="K40" t="n">
-        <v>0.156</v>
+        <v>0.173</v>
       </c>
       <c r="L40" t="n">
-        <v>-3.805</v>
+        <v>-6.671</v>
       </c>
       <c r="M40" t="n">
-        <v>0.0359</v>
+        <v>0.136</v>
       </c>
       <c r="N40" t="n">
-        <v>172.08</v>
+        <v>95.05</v>
       </c>
       <c r="O40" t="n">
         <v>4</v>
@@ -2790,7 +2790,7 @@
         <v>176579</v>
       </c>
       <c r="F43" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G43" t="n">
         <v>0.671</v>
@@ -2878,53 +2878,53 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Cross The Globe (feat. Juice WRLD)</t>
+          <t>Classy 101</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Almost Healed</t>
+          <t>Classy 101</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Lil Durk</t>
+          <t>Feid</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2023-05-26</t>
+          <t>2023-03-31</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>124905</v>
+        <v>195986</v>
       </c>
       <c r="F45" t="n">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="G45" t="n">
-        <v>0.743</v>
+        <v>0.859</v>
       </c>
       <c r="H45" t="n">
-        <v>0.0126</v>
+        <v>0.145</v>
       </c>
       <c r="I45" t="n">
-        <v>0.714</v>
+        <v>0.658</v>
       </c>
       <c r="J45" t="n">
         <v>0</v>
       </c>
       <c r="K45" t="n">
-        <v>0.0901</v>
+        <v>0.12</v>
       </c>
       <c r="L45" t="n">
-        <v>-6.024</v>
+        <v>-4.79</v>
       </c>
       <c r="M45" t="n">
-        <v>0.105</v>
+        <v>0.159</v>
       </c>
       <c r="N45" t="n">
-        <v>138.595</v>
+        <v>100.065</v>
       </c>
       <c r="O45" t="n">
         <v>4</v>
@@ -2933,53 +2933,53 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Classy 101</t>
+          <t>Like Crazy</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Classy 101</t>
+          <t>FACE</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Feid</t>
+          <t>Jimin</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-03-24</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>195986</v>
+        <v>212241</v>
       </c>
       <c r="F46" t="n">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G46" t="n">
-        <v>0.859</v>
+        <v>0.629</v>
       </c>
       <c r="H46" t="n">
-        <v>0.145</v>
+        <v>0.0025</v>
       </c>
       <c r="I46" t="n">
-        <v>0.658</v>
+        <v>0.733</v>
       </c>
       <c r="J46" t="n">
         <v>0</v>
       </c>
       <c r="K46" t="n">
-        <v>0.12</v>
+        <v>0.357</v>
       </c>
       <c r="L46" t="n">
-        <v>-4.79</v>
+        <v>-5.445</v>
       </c>
       <c r="M46" t="n">
-        <v>0.159</v>
+        <v>0.0419</v>
       </c>
       <c r="N46" t="n">
-        <v>100.065</v>
+        <v>120.001</v>
       </c>
       <c r="O46" t="n">
         <v>4</v>
@@ -2988,53 +2988,53 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>All My Life (feat. J. Cole)</t>
+          <t>Popular (with Playboi Carti &amp; Madonna) - The Idol Vol. 1 (Music from the HBO Original Series)</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Almost Healed</t>
+          <t>Popular [The Idol Vol. 1 (Music from the HBO Original Series)]</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Lil Durk</t>
+          <t>The Weeknd</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2023-05-26</t>
+          <t>2023-06-02</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>223878</v>
+        <v>215466</v>
       </c>
       <c r="F47" t="n">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="G47" t="n">
-        <v>0.787</v>
+        <v>0.852</v>
       </c>
       <c r="H47" t="n">
-        <v>0.0449</v>
+        <v>0.06519999999999999</v>
       </c>
       <c r="I47" t="n">
-        <v>0.57</v>
+        <v>0.675</v>
       </c>
       <c r="J47" t="n">
-        <v>0</v>
+        <v>3.74e-05</v>
       </c>
       <c r="K47" t="n">
-        <v>0.135</v>
+        <v>0.36</v>
       </c>
       <c r="L47" t="n">
-        <v>-5.881</v>
+        <v>-6.271</v>
       </c>
       <c r="M47" t="n">
-        <v>0.225</v>
+        <v>0.197</v>
       </c>
       <c r="N47" t="n">
-        <v>142.974</v>
+        <v>99.012</v>
       </c>
       <c r="O47" t="n">
         <v>4</v>
@@ -3208,53 +3208,53 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Like Crazy</t>
+          <t>Cross The Globe (feat. Juice WRLD)</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>FACE</t>
+          <t>Almost Healed</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Jimin</t>
+          <t>Lil Durk</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2023-03-24</t>
+          <t>2023-05-26</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>212241</v>
+        <v>124905</v>
       </c>
       <c r="F51" t="n">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="G51" t="n">
-        <v>0.629</v>
+        <v>0.743</v>
       </c>
       <c r="H51" t="n">
-        <v>0.0025</v>
+        <v>0.0126</v>
       </c>
       <c r="I51" t="n">
-        <v>0.733</v>
+        <v>0.714</v>
       </c>
       <c r="J51" t="n">
         <v>0</v>
       </c>
       <c r="K51" t="n">
-        <v>0.357</v>
+        <v>0.0901</v>
       </c>
       <c r="L51" t="n">
-        <v>-5.445</v>
+        <v>-6.024</v>
       </c>
       <c r="M51" t="n">
-        <v>0.0419</v>
+        <v>0.105</v>
       </c>
       <c r="N51" t="n">
-        <v>120.001</v>
+        <v>138.595</v>
       </c>
       <c r="O51" t="n">
         <v>4</v>

</xml_diff>